<commit_message>
Implemented CfgFindKey routine. Config file is now parsed and written into the connection menu.
</commit_message>
<xml_diff>
--- a/docs/cfg linked list.xlsx
+++ b/docs/cfg linked list.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\NXtel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54983F92-F3CD-497F-BC27-99C4B4803911}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3892E42A-D267-47C5-8F0C-4FD190219F49}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4530" xr2:uid="{51DC10E3-4471-42AC-8B64-0C732D71BB51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4530" activeTab="1" xr2:uid="{51DC10E3-4471-42AC-8B64-0C732D71BB51}"/>
   </bookViews>
   <sheets>
     <sheet name="CfgList" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Match" sheetId="3" r:id="rId2"/>
+    <sheet name="Compare" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Seq</t>
   </si>
@@ -127,6 +128,15 @@
   </si>
   <si>
     <t>0025</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>E32F</t>
+  </si>
+  <si>
+    <t>hl</t>
   </si>
 </sst>
 </file>
@@ -170,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -187,6 +197,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2818B63-B917-4D86-8AC5-33C25C0527ED}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
@@ -796,6 +809,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10FB405-DB3D-4675-8FC4-21CF4027DE48}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C8C417-D941-4AE6-8629-B7425F4798E8}">
   <dimension ref="A1:C11"/>
   <sheetViews>

</xml_diff>